<commit_message>
changement de medication.concept.coding en medication.concept 8960e7dc479911639e6d822ce31b1cf71675c89d
</commit_message>
<xml_diff>
--- a/update-mapping-pn13/ig/StructureDefinition-oncofair-medicationadministration-component.xlsx
+++ b/update-mapping-pn13/ig/StructureDefinition-oncofair-medicationadministration-component.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$66</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2597" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="454">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-14T09:45:22+00:00</t>
+    <t>2024-06-17T08:31:35+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -710,10 +710,7 @@
     <t>If only a code is specified, then it needs to be a code for a specific product. If more information is required, then the use of the medication resource is recommended.  For example, if you require form or lot number, then you must reference the Medication resource.</t>
   </si>
   <si>
-    <t>Codes identifying substance or product that can be administered.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/medication-codes</t>
+    <t>http://ltsi.univ-rennes.fr/ValueSet/concept-medication-oncofair-valueset</t>
   </si>
   <si>
     <t>Composant</t>
@@ -774,253 +771,197 @@
     <t>A reference to a concept - e.g. the information is identified by its general class to the degree of precision found in the terminology.</t>
   </si>
   <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;code value="component"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
+  </si>
+  <si>
     <t>CodeableReference.concept</t>
   </si>
   <si>
-    <t>MedicationAdministration.medication.concept.id</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.medication.concept.extension</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.medication.concept.coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding
+    <t>MedicationAdministration.medication.reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference
 </t>
   </si>
   <si>
-    <t>Code defined by a terminology system</t>
-  </si>
-  <si>
-    <t>A reference to a code defined by a terminology system.</t>
-  </si>
-  <si>
-    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
-  </si>
-  <si>
-    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
-  </si>
-  <si>
-    <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
-  &lt;code value="component"/&gt;
-&lt;/valueCoding&gt;</t>
-  </si>
-  <si>
-    <t>CodeableConcept.coding</t>
-  </si>
-  <si>
-    <t>union(., ./translation)</t>
-  </si>
-  <si>
-    <t>C*E.1-8, C*E.10-22</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.medication.concept.text</t>
+    <t>Reference to a resource (by instance)</t>
+  </si>
+  <si>
+    <t>A reference to a resource the provides exact details about the information being referenced.</t>
+  </si>
+  <si>
+    <t>CodeableReference.reference</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Patient|Group)
+</t>
+  </si>
+  <si>
+    <t>Who received medication</t>
+  </si>
+  <si>
+    <t>The person or animal or group receiving the medication.</t>
+  </si>
+  <si>
+    <t>Event.subject</t>
+  </si>
+  <si>
+    <t>FiveWs.subject[x]</t>
+  </si>
+  <si>
+    <t>.participation[typeCode=SBJ].role[classCode=PAT]</t>
+  </si>
+  <si>
+    <t>PID-3 Patient ID List</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.encounter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Encounter)
+</t>
+  </si>
+  <si>
+    <t>Encounter administered as part of</t>
+  </si>
+  <si>
+    <t>The visit, admission, or other contact between patient and health care provider during which the medication administration was performed.</t>
+  </si>
+  <si>
+    <t>Event.encounter</t>
+  </si>
+  <si>
+    <t>FiveWs.context</t>
+  </si>
+  <si>
+    <t>.inboundRelationship[typeCode=COMP].source[classCode=ENC, moodCode=EVN, code="type of encounter or episode"]</t>
+  </si>
+  <si>
+    <t>PV1-19 Visit Number</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.supportingInformation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Resource)
+</t>
+  </si>
+  <si>
+    <t>Additional information to support administration</t>
+  </si>
+  <si>
+    <t>Additional information (for example, patient height and weight) that supports the administration of the medication.  This attribute can be used to provide documentation of specific characteristics of the patient present at the time of administration.  For example, if the dose says "give "x" if the heartrate exceeds "y"", then the heart rate can be included using this attribute.</t>
+  </si>
+  <si>
+    <t>.outboundRelationship[typeCode=PERT].target[A_SupportingClinicalStatement CMET minimal with many different choices of classCodes(ORG, ENC, PROC, SPLY, SBADM, OBS) and each of the act class codes draws from one or more of the following moodCodes (EVN, DEF, INT PRMS, RQO, PRP, APT, ARQ, GOL)]</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.occurence[x]</t>
+  </si>
+  <si>
+    <t>dateTime
+PeriodTiming</t>
+  </si>
+  <si>
+    <t>Specific date/time or interval of time during which the administration took place (or did not take place)</t>
+  </si>
+  <si>
+    <t>A specific date/time or interval of time during which the administration took place (or did not take place). For many administrations, such as swallowing a tablet the use of dateTime is more appropriate.</t>
+  </si>
+  <si>
+    <t>Event.occurrence[x]</t>
+  </si>
+  <si>
+    <t>FiveWs.done[x]</t>
+  </si>
+  <si>
+    <t>.effectiveTime</t>
+  </si>
+  <si>
+    <t>RXA-3 Date/Time Start of Administration / RXA-4 Date/Time End of Administration</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.recorded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dateTime
+</t>
+  </si>
+  <si>
+    <t>When the MedicationAdministration was first captured in the subject's record</t>
+  </si>
+  <si>
+    <t>The date the occurrence of the  MedicationAdministration was first captured in the record - potentially significantly after the occurrence of the event.</t>
+  </si>
+  <si>
+    <t>FiveWs.recorded</t>
+  </si>
+  <si>
+    <t>.participation[typeCode=AUT].time</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.isSubPotent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean
+</t>
+  </si>
+  <si>
+    <t>Full dose was not administered</t>
+  </si>
+  <si>
+    <t>An indication that the full dose was not administered.</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.subPotentReason</t>
+  </si>
+  <si>
+    <t>Reason full dose was not administered</t>
+  </si>
+  <si>
+    <t>The reason or reasons why the full dose was not administered.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/administration-subpotent-reason</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.performer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BackboneElement
+</t>
+  </si>
+  <si>
+    <t>Who or what performed the medication administration and what type of performance they did</t>
+  </si>
+  <si>
+    <t>The performer of the medication treatment.  For devices this is the device that performed the administration of the medication.  An IV Pump would be an example of a device that is performing the administration. Both the IV Pump and the practitioner that set the rate or bolus on the pump can be listed as performers.</t>
+  </si>
+  <si>
+    <t>Event.performer</t>
+  </si>
+  <si>
+    <t>FiveWs.actor</t>
+  </si>
+  <si>
+    <t>.participation[typeCode=PRF]</t>
+  </si>
+  <si>
+    <t>RXA-10 Administering Provider / PRT-5 Participation Person: PRT-4 Participation='AP' (RXA-10 is deprecated)</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.performer.id</t>
   </si>
   <si>
     <t xml:space="preserve">string
 </t>
-  </si>
-  <si>
-    <t>Plain text representation of the concept</t>
-  </si>
-  <si>
-    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
-  </si>
-  <si>
-    <t>Very often the text is the same as a displayName of one of the codings.</t>
-  </si>
-  <si>
-    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
-  </si>
-  <si>
-    <t>CodeableConcept.text</t>
-  </si>
-  <si>
-    <t>./originalText[mediaType/code="text/plain"]/data</t>
-  </si>
-  <si>
-    <t>C*E.9. But note many systems use C*E.2 for this</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.medication.reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference
-</t>
-  </si>
-  <si>
-    <t>Reference to a resource (by instance)</t>
-  </si>
-  <si>
-    <t>A reference to a resource the provides exact details about the information being referenced.</t>
-  </si>
-  <si>
-    <t>CodeableReference.reference</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Patient|Group)
-</t>
-  </si>
-  <si>
-    <t>Who received medication</t>
-  </si>
-  <si>
-    <t>The person or animal or group receiving the medication.</t>
-  </si>
-  <si>
-    <t>Event.subject</t>
-  </si>
-  <si>
-    <t>FiveWs.subject[x]</t>
-  </si>
-  <si>
-    <t>.participation[typeCode=SBJ].role[classCode=PAT]</t>
-  </si>
-  <si>
-    <t>PID-3 Patient ID List</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.encounter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Encounter)
-</t>
-  </si>
-  <si>
-    <t>Encounter administered as part of</t>
-  </si>
-  <si>
-    <t>The visit, admission, or other contact between patient and health care provider during which the medication administration was performed.</t>
-  </si>
-  <si>
-    <t>Event.encounter</t>
-  </si>
-  <si>
-    <t>FiveWs.context</t>
-  </si>
-  <si>
-    <t>.inboundRelationship[typeCode=COMP].source[classCode=ENC, moodCode=EVN, code="type of encounter or episode"]</t>
-  </si>
-  <si>
-    <t>PV1-19 Visit Number</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.supportingInformation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Resource)
-</t>
-  </si>
-  <si>
-    <t>Additional information to support administration</t>
-  </si>
-  <si>
-    <t>Additional information (for example, patient height and weight) that supports the administration of the medication.  This attribute can be used to provide documentation of specific characteristics of the patient present at the time of administration.  For example, if the dose says "give "x" if the heartrate exceeds "y"", then the heart rate can be included using this attribute.</t>
-  </si>
-  <si>
-    <t>.outboundRelationship[typeCode=PERT].target[A_SupportingClinicalStatement CMET minimal with many different choices of classCodes(ORG, ENC, PROC, SPLY, SBADM, OBS) and each of the act class codes draws from one or more of the following moodCodes (EVN, DEF, INT PRMS, RQO, PRP, APT, ARQ, GOL)]</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.occurence[x]</t>
-  </si>
-  <si>
-    <t>dateTime
-PeriodTiming</t>
-  </si>
-  <si>
-    <t>Specific date/time or interval of time during which the administration took place (or did not take place)</t>
-  </si>
-  <si>
-    <t>A specific date/time or interval of time during which the administration took place (or did not take place). For many administrations, such as swallowing a tablet the use of dateTime is more appropriate.</t>
-  </si>
-  <si>
-    <t>Event.occurrence[x]</t>
-  </si>
-  <si>
-    <t>FiveWs.done[x]</t>
-  </si>
-  <si>
-    <t>.effectiveTime</t>
-  </si>
-  <si>
-    <t>RXA-3 Date/Time Start of Administration / RXA-4 Date/Time End of Administration</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.recorded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dateTime
-</t>
-  </si>
-  <si>
-    <t>When the MedicationAdministration was first captured in the subject's record</t>
-  </si>
-  <si>
-    <t>The date the occurrence of the  MedicationAdministration was first captured in the record - potentially significantly after the occurrence of the event.</t>
-  </si>
-  <si>
-    <t>FiveWs.recorded</t>
-  </si>
-  <si>
-    <t>.participation[typeCode=AUT].time</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.isSubPotent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boolean
-</t>
-  </si>
-  <si>
-    <t>Full dose was not administered</t>
-  </si>
-  <si>
-    <t>An indication that the full dose was not administered.</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.subPotentReason</t>
-  </si>
-  <si>
-    <t>Reason full dose was not administered</t>
-  </si>
-  <si>
-    <t>The reason or reasons why the full dose was not administered.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/administration-subpotent-reason</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.performer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BackboneElement
-</t>
-  </si>
-  <si>
-    <t>Who or what performed the medication administration and what type of performance they did</t>
-  </si>
-  <si>
-    <t>The performer of the medication treatment.  For devices this is the device that performed the administration of the medication.  An IV Pump would be an example of a device that is performing the administration. Both the IV Pump and the practitioner that set the rate or bolus on the pump can be listed as performers.</t>
-  </si>
-  <si>
-    <t>Event.performer</t>
-  </si>
-  <si>
-    <t>FiveWs.actor</t>
-  </si>
-  <si>
-    <t>.participation[typeCode=PRF]</t>
-  </si>
-  <si>
-    <t>RXA-10 Administering Provider / PRT-5 Participation Person: PRT-4 Participation='AP' (RXA-10 is deprecated)</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.performer.id</t>
   </si>
   <si>
     <t>MedicationAdministration.performer.extension</t>
@@ -1812,7 +1753,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO70"/>
+  <dimension ref="A1:AO66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1822,7 +1763,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="77.01171875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="52.77734375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="51.53515625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="43.3671875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
@@ -1846,7 +1787,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="124.42578125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="58.77734375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="66.98828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
@@ -4262,13 +4203,11 @@
         <v>76</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="Y21" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="Y21" s="2"/>
+      <c r="Z21" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="Z21" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="AA21" t="s" s="2">
         <v>76</v>
@@ -4301,27 +4240,27 @@
         <v>100</v>
       </c>
       <c r="AK21" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AL21" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="AL21" t="s" s="2">
+      <c r="AM21" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="AM21" t="s" s="2">
+      <c r="AN21" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="AN21" t="s" s="2">
+      <c r="AO21" t="s" s="2">
         <v>225</v>
-      </c>
-      <c r="AO21" t="s" s="2">
-        <v>226</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4347,10 +4286,10 @@
         <v>90</v>
       </c>
       <c r="L22" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="M22" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -4401,31 +4340,31 @@
         <v>76</v>
       </c>
       <c r="AF22" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="AG22" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH22" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="AI22" t="s" s="2">
         <v>230</v>
       </c>
-      <c r="AG22" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH22" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="AI22" t="s" s="2">
+      <c r="AJ22" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK22" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL22" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AM22" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN22" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="AJ22" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK22" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL22" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM22" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>76</v>
@@ -4433,10 +4372,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4462,10 +4401,10 @@
         <v>135</v>
       </c>
       <c r="L23" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="M23" t="s" s="2">
         <v>234</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>235</v>
       </c>
       <c r="N23" t="s" s="2">
         <v>165</v>
@@ -4509,7 +4448,7 @@
         <v>138</v>
       </c>
       <c r="AC23" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AD23" t="s" s="2">
         <v>76</v>
@@ -4518,7 +4457,7 @@
         <v>139</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>77</v>
@@ -4542,7 +4481,7 @@
         <v>76</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>76</v>
@@ -4550,10 +4489,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4579,10 +4518,10 @@
         <v>200</v>
       </c>
       <c r="L24" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="M24" t="s" s="2">
         <v>239</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>240</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -4594,7 +4533,7 @@
         <v>76</v>
       </c>
       <c r="S24" t="s" s="2">
-        <v>76</v>
+        <v>240</v>
       </c>
       <c r="T24" t="s" s="2">
         <v>76</v>
@@ -4688,16 +4627,16 @@
         <v>76</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>90</v>
+        <v>243</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -4748,7 +4687,7 @@
         <v>76</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>77</v>
@@ -4757,10 +4696,10 @@
         <v>88</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>231</v>
+        <v>76</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>76</v>
@@ -4772,7 +4711,7 @@
         <v>76</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>232</v>
+        <v>133</v>
       </c>
       <c r="AO25" t="s" s="2">
         <v>76</v>
@@ -4780,21 +4719,21 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>76</v>
@@ -4803,20 +4742,18 @@
         <v>76</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>135</v>
+        <v>248</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>165</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
         <v>76</v>
@@ -4853,54 +4790,54 @@
         <v>76</v>
       </c>
       <c r="AB26" t="s" s="2">
-        <v>138</v>
+        <v>76</v>
       </c>
       <c r="AC26" t="s" s="2">
-        <v>236</v>
+        <v>76</v>
       </c>
       <c r="AD26" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>139</v>
+        <v>76</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>76</v>
+        <v>251</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>76</v>
+        <v>252</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>232</v>
+        <v>253</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>76</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4911,7 +4848,7 @@
         <v>77</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>76</v>
@@ -4920,23 +4857,19 @@
         <v>76</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="O27" t="s" s="2">
-        <v>249</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
         <v>76</v>
       </c>
@@ -4945,7 +4878,7 @@
         <v>76</v>
       </c>
       <c r="S27" t="s" s="2">
-        <v>250</v>
+        <v>76</v>
       </c>
       <c r="T27" t="s" s="2">
         <v>76</v>
@@ -4984,13 +4917,13 @@
         <v>76</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>76</v>
@@ -5002,24 +4935,24 @@
         <v>76</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>76</v>
+        <v>259</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>76</v>
+        <v>260</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>253</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -5030,7 +4963,7 @@
         <v>77</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>76</v>
@@ -5039,23 +4972,19 @@
         <v>76</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="O28" t="s" s="2">
-        <v>259</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
         <v>76</v>
       </c>
@@ -5103,13 +5032,13 @@
         <v>76</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>76</v>
@@ -5124,21 +5053,21 @@
         <v>76</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>76</v>
+        <v>260</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>262</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5146,7 +5075,7 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>88</v>
@@ -5161,13 +5090,13 @@
         <v>89</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -5218,10 +5147,10 @@
         <v>76</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>88</v>
@@ -5236,24 +5165,24 @@
         <v>76</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>76</v>
+        <v>272</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>76</v>
+        <v>273</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>133</v>
+        <v>274</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>76</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5261,7 +5190,7 @@
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>88</v>
@@ -5276,13 +5205,13 @@
         <v>89</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -5333,10 +5262,10 @@
         <v>76</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>88</v>
@@ -5351,24 +5280,24 @@
         <v>76</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>272</v>
+        <v>76</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>275</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5391,13 +5320,13 @@
         <v>76</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -5448,7 +5377,7 @@
         <v>76</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>77</v>
@@ -5466,24 +5395,24 @@
         <v>76</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>280</v>
+        <v>76</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>281</v>
+        <v>76</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>282</v>
+        <v>76</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>283</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5506,13 +5435,13 @@
         <v>76</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>285</v>
+        <v>200</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5539,13 +5468,11 @@
         <v>76</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y32" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="Y32" s="2"/>
       <c r="Z32" t="s" s="2">
-        <v>76</v>
+        <v>289</v>
       </c>
       <c r="AA32" t="s" s="2">
         <v>76</v>
@@ -5563,7 +5490,7 @@
         <v>76</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>77</v>
@@ -5584,10 +5511,10 @@
         <v>76</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>281</v>
+        <v>76</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>288</v>
+        <v>76</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>76</v>
@@ -5595,10 +5522,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5606,10 +5533,10 @@
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>76</v>
@@ -5621,13 +5548,13 @@
         <v>89</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -5678,13 +5605,13 @@
         <v>76</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>76</v>
@@ -5696,24 +5623,24 @@
         <v>76</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5733,16 +5660,16 @@
         <v>76</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>299</v>
+        <v>227</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>300</v>
+        <v>228</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5793,7 +5720,7 @@
         <v>76</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>297</v>
+        <v>229</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>77</v>
@@ -5802,10 +5729,10 @@
         <v>88</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>76</v>
+        <v>230</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>76</v>
@@ -5814,10 +5741,10 @@
         <v>76</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>301</v>
+        <v>76</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>302</v>
+        <v>231</v>
       </c>
       <c r="AO34" t="s" s="2">
         <v>76</v>
@@ -5825,21 +5752,21 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>76</v>
@@ -5851,15 +5778,17 @@
         <v>76</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>304</v>
+        <v>135</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>305</v>
+        <v>233</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="N35" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>165</v>
+      </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
         <v>76</v>
@@ -5908,19 +5837,19 @@
         <v>76</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>303</v>
+        <v>236</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>76</v>
@@ -5932,7 +5861,7 @@
         <v>76</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>76</v>
+        <v>231</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>76</v>
@@ -5940,14 +5869,14 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
-        <v>76</v>
+        <v>302</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
@@ -5960,22 +5889,26 @@
         <v>76</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>200</v>
+        <v>135</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
+        <v>304</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="O36" t="s" s="2">
+        <v>166</v>
+      </c>
       <c r="P36" t="s" s="2">
         <v>76</v>
       </c>
@@ -5999,11 +5932,13 @@
         <v>76</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="Y36" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="Y36" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="Z36" t="s" s="2">
-        <v>310</v>
+        <v>76</v>
       </c>
       <c r="AA36" t="s" s="2">
         <v>76</v>
@@ -6021,7 +5956,7 @@
         <v>76</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>77</v>
@@ -6033,7 +5968,7 @@
         <v>76</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>76</v>
@@ -6045,7 +5980,7 @@
         <v>76</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>76</v>
+        <v>133</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>76</v>
@@ -6053,10 +5988,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6067,7 +6002,7 @@
         <v>77</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>76</v>
@@ -6076,16 +6011,16 @@
         <v>76</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>312</v>
+        <v>200</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -6112,13 +6047,13 @@
         <v>76</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>76</v>
+        <v>203</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>76</v>
+        <v>309</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>76</v>
+        <v>310</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>76</v>
@@ -6136,13 +6071,13 @@
         <v>76</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>76</v>
@@ -6154,24 +6089,24 @@
         <v>76</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>316</v>
+        <v>76</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="AO37" t="s" s="2">
-        <v>318</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6179,7 +6114,7 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>88</v>
@@ -6191,16 +6126,16 @@
         <v>76</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>255</v>
+        <v>314</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>228</v>
+        <v>315</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>229</v>
+        <v>316</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -6251,31 +6186,31 @@
         <v>76</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>230</v>
+        <v>313</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>88</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>231</v>
+        <v>76</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>76</v>
+        <v>317</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>232</v>
+        <v>318</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>76</v>
@@ -6283,14 +6218,14 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -6309,17 +6244,15 @@
         <v>76</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>135</v>
+        <v>320</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>234</v>
+        <v>321</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>165</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
         <v>76</v>
@@ -6344,13 +6277,13 @@
         <v>76</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>76</v>
+        <v>203</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>76</v>
+        <v>323</v>
       </c>
       <c r="Z39" t="s" s="2">
-        <v>76</v>
+        <v>324</v>
       </c>
       <c r="AA39" t="s" s="2">
         <v>76</v>
@@ -6368,7 +6301,7 @@
         <v>76</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>237</v>
+        <v>319</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>77</v>
@@ -6380,66 +6313,64 @@
         <v>76</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>76</v>
+        <v>325</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>232</v>
+        <v>326</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>76</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>322</v>
+        <v>76</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>135</v>
+        <v>329</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="O40" t="s" s="2">
-        <v>166</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
         <v>76</v>
       </c>
@@ -6487,42 +6418,42 @@
         <v>76</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>76</v>
+        <v>333</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>133</v>
+        <v>334</v>
       </c>
       <c r="AO40" t="s" s="2">
-        <v>76</v>
+        <v>335</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6533,7 +6464,7 @@
         <v>77</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>76</v>
@@ -6545,13 +6476,13 @@
         <v>76</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>200</v>
+        <v>337</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6578,13 +6509,13 @@
         <v>76</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>203</v>
+        <v>76</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>329</v>
+        <v>76</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>330</v>
+        <v>76</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>76</v>
@@ -6602,13 +6533,13 @@
         <v>76</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="AI41" t="s" s="2">
         <v>76</v>
@@ -6620,24 +6551,24 @@
         <v>76</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>331</v>
+        <v>76</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>76</v>
+        <v>341</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6645,28 +6576,28 @@
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H42" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="I42" t="s" s="2">
         <v>76</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -6705,25 +6636,23 @@
         <v>76</v>
       </c>
       <c r="AB42" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC42" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="AC42" s="2"/>
       <c r="AD42" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>76</v>
+        <v>139</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>76</v>
@@ -6735,13 +6664,13 @@
         <v>76</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>76</v>
@@ -6749,12 +6678,14 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>339</v>
-      </c>
-      <c r="C43" s="2"/>
+        <v>342</v>
+      </c>
+      <c r="C43" t="s" s="2">
+        <v>350</v>
+      </c>
       <c r="D43" t="s" s="2">
         <v>76</v>
       </c>
@@ -6763,7 +6694,7 @@
         <v>77</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>76</v>
@@ -6775,13 +6706,13 @@
         <v>76</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6808,13 +6739,13 @@
         <v>76</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>203</v>
+        <v>76</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>343</v>
+        <v>76</v>
       </c>
       <c r="Z43" t="s" s="2">
-        <v>344</v>
+        <v>76</v>
       </c>
       <c r="AA43" t="s" s="2">
         <v>76</v>
@@ -6832,7 +6763,7 @@
         <v>76</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>77</v>
@@ -6847,27 +6778,27 @@
         <v>100</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>76</v>
+        <v>352</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>347</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6875,7 +6806,7 @@
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>88</v>
@@ -6890,17 +6821,15 @@
         <v>76</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>349</v>
+        <v>90</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>350</v>
+        <v>227</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>352</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
         <v>76</v>
@@ -6910,7 +6839,7 @@
         <v>76</v>
       </c>
       <c r="S44" t="s" s="2">
-        <v>76</v>
+        <v>350</v>
       </c>
       <c r="T44" t="s" s="2">
         <v>76</v>
@@ -6949,7 +6878,7 @@
         <v>76</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>348</v>
+        <v>229</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>77</v>
@@ -6958,37 +6887,37 @@
         <v>88</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>76</v>
+        <v>230</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>353</v>
+        <v>76</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>354</v>
+        <v>231</v>
       </c>
       <c r="AO44" t="s" s="2">
-        <v>355</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B45" t="s" s="2">
         <v>356</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
@@ -7007,15 +6936,17 @@
         <v>76</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>357</v>
+        <v>135</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>358</v>
+        <v>233</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="N45" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>165</v>
+      </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
         <v>76</v>
@@ -7052,19 +6983,19 @@
         <v>76</v>
       </c>
       <c r="AB45" t="s" s="2">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="AC45" t="s" s="2">
-        <v>76</v>
+        <v>235</v>
       </c>
       <c r="AD45" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>76</v>
+        <v>139</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>356</v>
+        <v>236</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>77</v>
@@ -7076,7 +7007,7 @@
         <v>76</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>76</v>
@@ -7088,18 +7019,18 @@
         <v>76</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>360</v>
+        <v>231</v>
       </c>
       <c r="AO45" t="s" s="2">
-        <v>361</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7110,27 +7041,29 @@
         <v>77</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H46" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I46" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J46" t="s" s="2">
         <v>89</v>
       </c>
-      <c r="I46" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J46" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="K46" t="s" s="2">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>365</v>
-      </c>
-      <c r="N46" s="2"/>
+        <v>361</v>
+      </c>
+      <c r="N46" t="s" s="2">
+        <v>362</v>
+      </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
         <v>76</v>
@@ -7167,23 +7100,25 @@
         <v>76</v>
       </c>
       <c r="AB46" t="s" s="2">
-        <v>366</v>
-      </c>
-      <c r="AC46" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="AD46" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>139</v>
+        <v>76</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>76</v>
@@ -7195,28 +7130,26 @@
         <v>76</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>367</v>
+        <v>76</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="AO46" t="s" s="2">
-        <v>76</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>362</v>
-      </c>
-      <c r="C47" t="s" s="2">
-        <v>370</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
         <v>76</v>
       </c>
@@ -7234,16 +7167,16 @@
         <v>76</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>363</v>
+        <v>277</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -7294,13 +7227,13 @@
         <v>76</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>76</v>
@@ -7309,27 +7242,27 @@
         <v>100</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>372</v>
+        <v>76</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>367</v>
+        <v>76</v>
       </c>
       <c r="AM47" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AO47" t="s" s="2">
-        <v>76</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7349,16 +7282,16 @@
         <v>76</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>90</v>
+        <v>373</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>228</v>
+        <v>374</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>229</v>
+        <v>375</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7370,7 +7303,7 @@
         <v>76</v>
       </c>
       <c r="S48" t="s" s="2">
-        <v>370</v>
+        <v>76</v>
       </c>
       <c r="T48" t="s" s="2">
         <v>76</v>
@@ -7409,19 +7342,19 @@
         <v>76</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>230</v>
+        <v>376</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>88</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>231</v>
+        <v>76</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>76</v>
@@ -7433,29 +7366,31 @@
         <v>76</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>232</v>
+        <v>377</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>76</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>376</v>
-      </c>
-      <c r="C49" s="2"/>
+        <v>342</v>
+      </c>
+      <c r="C49" t="s" s="2">
+        <v>379</v>
+      </c>
       <c r="D49" t="s" s="2">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>76</v>
@@ -7467,17 +7402,15 @@
         <v>76</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>135</v>
+        <v>343</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>234</v>
+        <v>380</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>165</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="N49" s="2"/>
       <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
         <v>76</v>
@@ -7514,19 +7447,19 @@
         <v>76</v>
       </c>
       <c r="AB49" t="s" s="2">
-        <v>138</v>
+        <v>76</v>
       </c>
       <c r="AC49" t="s" s="2">
-        <v>236</v>
+        <v>76</v>
       </c>
       <c r="AD49" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>139</v>
+        <v>76</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>237</v>
+        <v>342</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>77</v>
@@ -7538,19 +7471,19 @@
         <v>76</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>76</v>
+        <v>381</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>76</v>
+        <v>347</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>232</v>
+        <v>348</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>76</v>
@@ -7558,10 +7491,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7569,7 +7502,7 @@
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>88</v>
@@ -7581,20 +7514,18 @@
         <v>76</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>379</v>
+        <v>90</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>380</v>
+        <v>227</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>382</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="N50" s="2"/>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
         <v>76</v>
@@ -7604,7 +7535,7 @@
         <v>76</v>
       </c>
       <c r="S50" t="s" s="2">
-        <v>76</v>
+        <v>379</v>
       </c>
       <c r="T50" t="s" s="2">
         <v>76</v>
@@ -7643,7 +7574,7 @@
         <v>76</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>383</v>
+        <v>229</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>77</v>
@@ -7652,10 +7583,10 @@
         <v>88</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>76</v>
+        <v>230</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>76</v>
@@ -7667,29 +7598,29 @@
         <v>76</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>133</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>386</v>
+        <v>356</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>76</v>
@@ -7698,18 +7629,20 @@
         <v>76</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>298</v>
+        <v>135</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>387</v>
+        <v>233</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="N51" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>165</v>
+      </c>
       <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
         <v>76</v>
@@ -7746,31 +7679,31 @@
         <v>76</v>
       </c>
       <c r="AB51" t="s" s="2">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="AC51" t="s" s="2">
-        <v>76</v>
+        <v>235</v>
       </c>
       <c r="AD51" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>76</v>
+        <v>139</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>76</v>
@@ -7782,18 +7715,18 @@
         <v>76</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>390</v>
+        <v>231</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>133</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>392</v>
+        <v>358</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7801,7 +7734,7 @@
       </c>
       <c r="E52" s="2"/>
       <c r="F52" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>88</v>
@@ -7816,15 +7749,17 @@
         <v>89</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>393</v>
+        <v>359</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>394</v>
+        <v>360</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="N52" s="2"/>
+        <v>361</v>
+      </c>
+      <c r="N52" t="s" s="2">
+        <v>362</v>
+      </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
         <v>76</v>
@@ -7873,10 +7808,10 @@
         <v>76</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>396</v>
+        <v>363</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>88</v>
@@ -7897,7 +7832,7 @@
         <v>76</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>397</v>
+        <v>364</v>
       </c>
       <c r="AO52" t="s" s="2">
         <v>133</v>
@@ -7905,14 +7840,12 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>362</v>
-      </c>
-      <c r="C53" t="s" s="2">
-        <v>399</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
         <v>76</v>
       </c>
@@ -7930,16 +7863,16 @@
         <v>76</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>363</v>
+        <v>277</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>400</v>
+        <v>367</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -7990,13 +7923,13 @@
         <v>76</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH53" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AI53" t="s" s="2">
         <v>76</v>
@@ -8005,27 +7938,27 @@
         <v>100</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>401</v>
+        <v>76</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>367</v>
+        <v>76</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>76</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8045,16 +7978,16 @@
         <v>76</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>90</v>
+        <v>373</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>228</v>
+        <v>374</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>229</v>
+        <v>375</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -8066,7 +7999,7 @@
         <v>76</v>
       </c>
       <c r="S54" t="s" s="2">
-        <v>399</v>
+        <v>76</v>
       </c>
       <c r="T54" t="s" s="2">
         <v>76</v>
@@ -8105,19 +8038,19 @@
         <v>76</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>230</v>
+        <v>376</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="AH54" t="s" s="2">
         <v>88</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>231</v>
+        <v>76</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="AK54" t="s" s="2">
         <v>76</v>
@@ -8129,32 +8062,32 @@
         <v>76</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>232</v>
+        <v>377</v>
       </c>
       <c r="AO54" t="s" s="2">
-        <v>76</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H55" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="I55" t="s" s="2">
         <v>76</v>
@@ -8163,17 +8096,15 @@
         <v>76</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>135</v>
+        <v>291</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>234</v>
+        <v>388</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>165</v>
-      </c>
+        <v>389</v>
+      </c>
+      <c r="N55" s="2"/>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
         <v>76</v>
@@ -8210,31 +8141,31 @@
         <v>76</v>
       </c>
       <c r="AB55" t="s" s="2">
-        <v>138</v>
+        <v>76</v>
       </c>
       <c r="AC55" t="s" s="2">
-        <v>236</v>
+        <v>76</v>
       </c>
       <c r="AD55" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>139</v>
+        <v>76</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>237</v>
+        <v>387</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>141</v>
+        <v>390</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>76</v>
@@ -8246,7 +8177,7 @@
         <v>76</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>232</v>
+        <v>391</v>
       </c>
       <c r="AO55" t="s" s="2">
         <v>76</v>
@@ -8254,10 +8185,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8277,20 +8208,18 @@
         <v>76</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>379</v>
+        <v>299</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>380</v>
+        <v>227</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>382</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="N56" s="2"/>
       <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
         <v>76</v>
@@ -8339,7 +8268,7 @@
         <v>76</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>383</v>
+        <v>229</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>77</v>
@@ -8348,10 +8277,10 @@
         <v>88</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>76</v>
+        <v>230</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="AK56" t="s" s="2">
         <v>76</v>
@@ -8363,29 +8292,29 @@
         <v>76</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="AO56" t="s" s="2">
-        <v>133</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H57" t="s" s="2">
         <v>76</v>
@@ -8394,18 +8323,20 @@
         <v>76</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>298</v>
+        <v>135</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>387</v>
+        <v>233</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="N57" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="N57" t="s" s="2">
+        <v>165</v>
+      </c>
       <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
         <v>76</v>
@@ -8454,19 +8385,19 @@
         <v>76</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH57" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="AI57" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="AK57" t="s" s="2">
         <v>76</v>
@@ -8478,50 +8409,54 @@
         <v>76</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>390</v>
+        <v>231</v>
       </c>
       <c r="AO57" t="s" s="2">
-        <v>133</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
-        <v>76</v>
+        <v>302</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="J58" t="s" s="2">
         <v>89</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>393</v>
+        <v>135</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>394</v>
+        <v>303</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="N58" s="2"/>
-      <c r="O58" s="2"/>
+        <v>304</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="O58" t="s" s="2">
+        <v>166</v>
+      </c>
       <c r="P58" t="s" s="2">
         <v>76</v>
       </c>
@@ -8569,19 +8504,19 @@
         <v>76</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>396</v>
+        <v>305</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="AK58" t="s" s="2">
         <v>76</v>
@@ -8593,18 +8528,18 @@
         <v>76</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>397</v>
+        <v>133</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>133</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8612,13 +8547,13 @@
       </c>
       <c r="E59" s="2"/>
       <c r="F59" t="s" s="2">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>88</v>
       </c>
       <c r="H59" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="I59" t="s" s="2">
         <v>76</v>
@@ -8627,13 +8562,13 @@
         <v>76</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -8684,7 +8619,7 @@
         <v>76</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>77</v>
@@ -8693,10 +8628,10 @@
         <v>88</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>76</v>
+        <v>398</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>410</v>
+        <v>100</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>76</v>
@@ -8708,7 +8643,7 @@
         <v>76</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="AO59" t="s" s="2">
         <v>76</v>
@@ -8716,10 +8651,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8742,15 +8677,17 @@
         <v>76</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>255</v>
+        <v>200</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>228</v>
+        <v>401</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="N60" s="2"/>
+        <v>402</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>403</v>
+      </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
         <v>76</v>
@@ -8775,13 +8712,13 @@
         <v>76</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>76</v>
+        <v>203</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>76</v>
+        <v>404</v>
       </c>
       <c r="Z60" t="s" s="2">
-        <v>76</v>
+        <v>405</v>
       </c>
       <c r="AA60" t="s" s="2">
         <v>76</v>
@@ -8799,7 +8736,7 @@
         <v>76</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>230</v>
+        <v>400</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>77</v>
@@ -8808,10 +8745,10 @@
         <v>88</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>231</v>
+        <v>76</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>76</v>
@@ -8823,29 +8760,29 @@
         <v>76</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>232</v>
+        <v>406</v>
       </c>
       <c r="AO60" t="s" s="2">
-        <v>76</v>
+        <v>407</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G61" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H61" t="s" s="2">
         <v>76</v>
@@ -8857,17 +8794,15 @@
         <v>76</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>135</v>
+        <v>200</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>234</v>
+        <v>409</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>165</v>
-      </c>
+        <v>410</v>
+      </c>
+      <c r="N61" s="2"/>
       <c r="O61" s="2"/>
       <c r="P61" t="s" s="2">
         <v>76</v>
@@ -8892,13 +8827,13 @@
         <v>76</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>76</v>
+        <v>203</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>76</v>
+        <v>411</v>
       </c>
       <c r="Z61" t="s" s="2">
-        <v>76</v>
+        <v>412</v>
       </c>
       <c r="AA61" t="s" s="2">
         <v>76</v>
@@ -8916,19 +8851,19 @@
         <v>76</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>237</v>
+        <v>408</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH61" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AI61" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>76</v>
@@ -8940,54 +8875,52 @@
         <v>76</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>232</v>
+        <v>413</v>
       </c>
       <c r="AO61" t="s" s="2">
-        <v>76</v>
+        <v>414</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
-        <v>322</v>
+        <v>76</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G62" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H62" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I62" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>135</v>
+        <v>200</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>323</v>
+        <v>416</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>324</v>
+        <v>417</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="O62" t="s" s="2">
-        <v>166</v>
-      </c>
+        <v>418</v>
+      </c>
+      <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
         <v>76</v>
       </c>
@@ -9011,13 +8944,13 @@
         <v>76</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>76</v>
+        <v>203</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>76</v>
+        <v>419</v>
       </c>
       <c r="Z62" t="s" s="2">
-        <v>76</v>
+        <v>420</v>
       </c>
       <c r="AA62" t="s" s="2">
         <v>76</v>
@@ -9035,19 +8968,19 @@
         <v>76</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>325</v>
+        <v>415</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH62" t="s" s="2">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AI62" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="AK62" t="s" s="2">
         <v>76</v>
@@ -9059,18 +8992,18 @@
         <v>76</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>133</v>
+        <v>421</v>
       </c>
       <c r="AO62" t="s" s="2">
-        <v>76</v>
+        <v>422</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>415</v>
+        <v>423</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>415</v>
+        <v>423</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9078,7 +9011,7 @@
       </c>
       <c r="E63" s="2"/>
       <c r="F63" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G63" t="s" s="2">
         <v>88</v>
@@ -9093,15 +9026,17 @@
         <v>76</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>255</v>
+        <v>424</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>417</v>
-      </c>
-      <c r="N63" s="2"/>
+        <v>426</v>
+      </c>
+      <c r="N63" t="s" s="2">
+        <v>427</v>
+      </c>
       <c r="O63" s="2"/>
       <c r="P63" t="s" s="2">
         <v>76</v>
@@ -9150,7 +9085,7 @@
         <v>76</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>415</v>
+        <v>423</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>77</v>
@@ -9159,13 +9094,13 @@
         <v>88</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>418</v>
+        <v>398</v>
       </c>
       <c r="AJ63" t="s" s="2">
         <v>100</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>76</v>
+        <v>428</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>76</v>
@@ -9174,18 +9109,18 @@
         <v>76</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>419</v>
+        <v>429</v>
       </c>
       <c r="AO63" t="s" s="2">
-        <v>76</v>
+        <v>430</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9193,7 +9128,7 @@
       </c>
       <c r="E64" s="2"/>
       <c r="F64" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>88</v>
@@ -9208,16 +9143,16 @@
         <v>76</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>200</v>
+        <v>424</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="N64" t="s" s="2">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
@@ -9243,31 +9178,29 @@
         <v>76</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>203</v>
+        <v>76</v>
       </c>
       <c r="Y64" t="s" s="2">
-        <v>424</v>
+        <v>76</v>
       </c>
       <c r="Z64" t="s" s="2">
-        <v>425</v>
+        <v>76</v>
       </c>
       <c r="AA64" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AB64" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC64" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>435</v>
+      </c>
+      <c r="AC64" s="2"/>
       <c r="AD64" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>76</v>
+        <v>436</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>77</v>
@@ -9276,7 +9209,7 @@
         <v>88</v>
       </c>
       <c r="AI64" t="s" s="2">
-        <v>76</v>
+        <v>398</v>
       </c>
       <c r="AJ64" t="s" s="2">
         <v>100</v>
@@ -9291,32 +9224,34 @@
         <v>76</v>
       </c>
       <c r="AN64" t="s" s="2">
-        <v>426</v>
+        <v>437</v>
       </c>
       <c r="AO64" t="s" s="2">
-        <v>427</v>
+        <v>438</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>428</v>
+        <v>439</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>428</v>
-      </c>
-      <c r="C65" s="2"/>
+        <v>431</v>
+      </c>
+      <c r="C65" t="s" s="2">
+        <v>440</v>
+      </c>
       <c r="D65" t="s" s="2">
         <v>76</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G65" t="s" s="2">
         <v>88</v>
       </c>
       <c r="H65" t="s" s="2">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="I65" t="s" s="2">
         <v>76</v>
@@ -9325,15 +9260,17 @@
         <v>76</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>200</v>
+        <v>424</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>430</v>
-      </c>
-      <c r="N65" s="2"/>
+        <v>442</v>
+      </c>
+      <c r="N65" t="s" s="2">
+        <v>443</v>
+      </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
         <v>76</v>
@@ -9358,32 +9295,32 @@
         <v>76</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>203</v>
+        <v>76</v>
       </c>
       <c r="Y65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF65" t="s" s="2">
         <v>431</v>
       </c>
-      <c r="Z65" t="s" s="2">
-        <v>432</v>
-      </c>
-      <c r="AA65" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB65" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC65" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD65" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE65" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF65" t="s" s="2">
-        <v>428</v>
-      </c>
       <c r="AG65" t="s" s="2">
         <v>77</v>
       </c>
@@ -9394,10 +9331,10 @@
         <v>76</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>100</v>
+        <v>444</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>76</v>
+        <v>445</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>76</v>
@@ -9406,18 +9343,18 @@
         <v>76</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>433</v>
+        <v>446</v>
       </c>
       <c r="AO65" t="s" s="2">
-        <v>434</v>
+        <v>447</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9428,7 +9365,7 @@
         <v>77</v>
       </c>
       <c r="G66" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H66" t="s" s="2">
         <v>76</v>
@@ -9440,16 +9377,16 @@
         <v>76</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>200</v>
+        <v>449</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>437</v>
+        <v>451</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="O66" s="2"/>
       <c r="P66" t="s" s="2">
@@ -9475,13 +9412,13 @@
         <v>76</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>203</v>
+        <v>76</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>439</v>
+        <v>76</v>
       </c>
       <c r="Z66" t="s" s="2">
-        <v>440</v>
+        <v>76</v>
       </c>
       <c r="AA66" t="s" s="2">
         <v>76</v>
@@ -9499,13 +9436,13 @@
         <v>76</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH66" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="AI66" t="s" s="2">
         <v>76</v>
@@ -9523,482 +9460,14 @@
         <v>76</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="AO66" t="s" s="2">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="67" hidden="true">
-      <c r="A67" t="s" s="2">
-        <v>443</v>
-      </c>
-      <c r="B67" t="s" s="2">
-        <v>443</v>
-      </c>
-      <c r="C67" s="2"/>
-      <c r="D67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E67" s="2"/>
-      <c r="F67" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="G67" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="H67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K67" t="s" s="2">
-        <v>444</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>445</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>446</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>447</v>
-      </c>
-      <c r="O67" s="2"/>
-      <c r="P67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q67" s="2"/>
-      <c r="R67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF67" t="s" s="2">
-        <v>443</v>
-      </c>
-      <c r="AG67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH67" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="AI67" t="s" s="2">
-        <v>418</v>
-      </c>
-      <c r="AJ67" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AK67" t="s" s="2">
-        <v>448</v>
-      </c>
-      <c r="AL67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM67" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN67" t="s" s="2">
-        <v>449</v>
-      </c>
-      <c r="AO67" t="s" s="2">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="68" hidden="true">
-      <c r="A68" t="s" s="2">
-        <v>451</v>
-      </c>
-      <c r="B68" t="s" s="2">
-        <v>451</v>
-      </c>
-      <c r="C68" s="2"/>
-      <c r="D68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E68" s="2"/>
-      <c r="F68" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="G68" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="H68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K68" t="s" s="2">
-        <v>444</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>452</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>453</v>
-      </c>
-      <c r="N68" t="s" s="2">
-        <v>454</v>
-      </c>
-      <c r="O68" s="2"/>
-      <c r="P68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q68" s="2"/>
-      <c r="R68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB68" t="s" s="2">
-        <v>455</v>
-      </c>
-      <c r="AC68" s="2"/>
-      <c r="AD68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE68" t="s" s="2">
-        <v>456</v>
-      </c>
-      <c r="AF68" t="s" s="2">
-        <v>451</v>
-      </c>
-      <c r="AG68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH68" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="AI68" t="s" s="2">
-        <v>418</v>
-      </c>
-      <c r="AJ68" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AK68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN68" t="s" s="2">
-        <v>457</v>
-      </c>
-      <c r="AO68" t="s" s="2">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="69" hidden="true">
-      <c r="A69" t="s" s="2">
-        <v>459</v>
-      </c>
-      <c r="B69" t="s" s="2">
-        <v>451</v>
-      </c>
-      <c r="C69" t="s" s="2">
-        <v>460</v>
-      </c>
-      <c r="D69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E69" s="2"/>
-      <c r="F69" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="G69" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="H69" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="I69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K69" t="s" s="2">
-        <v>444</v>
-      </c>
-      <c r="L69" t="s" s="2">
-        <v>461</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>462</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>463</v>
-      </c>
-      <c r="O69" s="2"/>
-      <c r="P69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q69" s="2"/>
-      <c r="R69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF69" t="s" s="2">
-        <v>451</v>
-      </c>
-      <c r="AG69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH69" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="AI69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AJ69" t="s" s="2">
-        <v>464</v>
-      </c>
-      <c r="AK69" t="s" s="2">
-        <v>465</v>
-      </c>
-      <c r="AL69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN69" t="s" s="2">
-        <v>466</v>
-      </c>
-      <c r="AO69" t="s" s="2">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="70" hidden="true">
-      <c r="A70" t="s" s="2">
-        <v>468</v>
-      </c>
-      <c r="B70" t="s" s="2">
-        <v>468</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E70" s="2"/>
-      <c r="F70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="G70" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K70" t="s" s="2">
-        <v>469</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>470</v>
-      </c>
-      <c r="M70" t="s" s="2">
-        <v>471</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>472</v>
-      </c>
-      <c r="O70" s="2"/>
-      <c r="P70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q70" s="2"/>
-      <c r="R70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF70" t="s" s="2">
-        <v>468</v>
-      </c>
-      <c r="AG70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH70" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AJ70" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AK70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN70" t="s" s="2">
-        <v>473</v>
-      </c>
-      <c r="AO70" t="s" s="2">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO70">
+  <autoFilter ref="A1:AO66">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10008,7 +9477,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI69">
+  <conditionalFormatting sqref="A2:AI65">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>